<commit_message>
Se renombra la carpeta ReadActivity por WriteActivity
</commit_message>
<xml_diff>
--- a/WordActivity/Resources/dataKichua.xlsx
+++ b/WordActivity/Resources/dataKichua.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>alejandro sanz no es lo mismo</t>
   </si>
@@ -33,10 +33,10 @@
     <t>Nivel</t>
   </si>
   <si>
-    <t>Eres,tanta,gente,quién,ahora</t>
-  </si>
-  <si>
-    <t>Eres,ahora</t>
+    <t>Eres - heres,tanta,gente,quién,ahora - ajora</t>
+  </si>
+  <si>
+    <t>Eres - heres,ahora - ajora</t>
   </si>
 </sst>
 </file>
@@ -405,17 +405,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -445,6 +445,20 @@
       </c>
       <c r="D2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>